<commit_message>
clean and timesheet update
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>Person</t>
   </si>
@@ -439,7 +439,7 @@
   <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -529,8 +529,15 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3">
+        <v>13.1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="E6" s="4"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>

</xml_diff>

<commit_message>
Added a ton of new domain objects, created abstraction for Dal, moved definition for UserManager and SignInManager, started integrating User objects with regular Domain objects.
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="9">
   <si>
     <t>Person</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>8h</t>
+  </si>
+  <si>
+    <t>5h</t>
   </si>
 </sst>
 </file>
@@ -439,7 +442,7 @@
   <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -544,40 +547,75 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>14.1</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="E7" s="4"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3">
+        <v>15.1</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E8" s="4"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3">
+        <v>15.1</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E9" s="4"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3">
+        <v>15.1</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="E10" s="4"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="E11" s="4"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>

</xml_diff>